<commit_message>
Add model, update figs
</commit_message>
<xml_diff>
--- a/SpeciesList.xlsx
+++ b/SpeciesList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d03c6ea88daad3e/Documenten/Shimoni/DATA/R/Github/Herbivory/Herbivory grazing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{49E64A2A-F09F-415E-B5B2-92F77E99242A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{E75523DB-91D8-4669-BDF7-08CF80C4D3BF}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{49E64A2A-F09F-415E-B5B2-92F77E99242A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{3887850C-3564-4BFF-8ABB-1B7BAEFD94CE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6879F9F5-B567-437C-A91B-69A6065869AF}"/>
   </bookViews>
@@ -1600,13 +1600,7 @@
     <t>#991d1f</t>
   </si>
   <si>
-    <t>#f8ef6a</t>
-  </si>
-  <si>
     <t>#dfd20b</t>
-  </si>
-  <si>
-    <t>#d0c40a</t>
   </si>
   <si>
     <t>#c1b609</t>
@@ -1616,6 +1610,12 @@
   </si>
   <si>
     <t>#3f65d4</t>
+  </si>
+  <si>
+    <t>#fff77d</t>
+  </si>
+  <si>
+    <t>#baaf00</t>
   </si>
 </sst>
 </file>
@@ -2094,8 +2094,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:O299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A271" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G300" sqref="G300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2181,7 +2181,7 @@
         <v>342</v>
       </c>
       <c r="G2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>358</v>
@@ -2226,7 +2226,7 @@
         <v>342</v>
       </c>
       <c r="G3" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>358</v>
@@ -3644,7 +3644,7 @@
         <v>342</v>
       </c>
       <c r="G35" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>358</v>
@@ -3685,7 +3685,7 @@
         <v>342</v>
       </c>
       <c r="G36" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J36" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3724,7 +3724,7 @@
         <v>342</v>
       </c>
       <c r="G37" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>358</v>
@@ -3769,7 +3769,7 @@
         <v>342</v>
       </c>
       <c r="G38" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H38" t="s">
         <v>358</v>
@@ -14714,7 +14714,7 @@
         <v>340</v>
       </c>
       <c r="G294" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="H294" s="8" t="s">
         <v>358</v>
@@ -14759,7 +14759,7 @@
         <v>342</v>
       </c>
       <c r="G295" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H295" s="1" t="s">
         <v>358</v>
@@ -14803,7 +14803,7 @@
         <v>342</v>
       </c>
       <c r="G296" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J296" s="10" t="str">
         <f t="shared" si="4"/>
@@ -14846,7 +14846,7 @@
         <v>342</v>
       </c>
       <c r="G297" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H297" s="1" t="s">
         <v>358</v>
@@ -14894,7 +14894,7 @@
         <v>340</v>
       </c>
       <c r="G298" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="H298" s="1" t="s">
         <v>358</v>
@@ -14939,7 +14939,7 @@
         <v>340</v>
       </c>
       <c r="G299" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H299" s="1" t="s">
         <v>358</v>

</xml_diff>